<commit_message>
update to test cases, changes
</commit_message>
<xml_diff>
--- a/Diseño y ejecucion/reporteIncidencias (1).xlsx
+++ b/Diseño y ejecucion/reporteIncidencias (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudio\Documents\QA\Trabajos QA\QAProject\ReporteIncidencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudio\Documents\QA\Trabajos QA\QAProject\Diseño y ejecucion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -145,9 +145,6 @@
 Status code 403 o 405</t>
   </si>
   <si>
-    <t>CP006-Agregar una nueva mascota</t>
-  </si>
-  <si>
     <t>El status code no es el correcto</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t xml:space="preserve">Actualizar los datos de una mascotautilizando un Id que no existe </t>
   </si>
   <si>
-    <t>CP021- Actualizar informacion de una mascota</t>
-  </si>
-  <si>
     <t>1. Ingrese a Postman
 2. Abra una solicitud PUT
 3.Ingresa la URL /pet
@@ -334,16 +328,10 @@
 6.Click en Send Btn.</t>
   </si>
   <si>
-    <t>CP013- Filtrar mascotas por ID</t>
-  </si>
-  <si>
     <t>Si el estado es incorrecto se debe mostrar status code 400 invalid status value</t>
   </si>
   <si>
     <t xml:space="preserve">Al filtrar mascota por un Id que no e creado debe de aparecer un status code invalido </t>
-  </si>
-  <si>
-    <t>CP011- Filtrar mascota por Status</t>
   </si>
   <si>
     <t xml:space="preserve">realizara la filtracion pos status de la mascota
@@ -352,9 +340,6 @@
   </si>
   <si>
     <t>Al filtrar la mascota por un estado invalido debe de mostrar error</t>
-  </si>
-  <si>
-    <t>CP012- Filtrar mascota por Status</t>
   </si>
   <si>
     <t>Al filtrar la mascota por un estado vacio debe de mostrar error</t>
@@ -379,9 +364,6 @@
 4. Dar click en "findByStatus" dejando vacio
 5.Selecionar una opcion
 6.Click en Send Btn.</t>
-  </si>
-  <si>
-    <t>CP025-Actualizar una mascota en la tienda con datos del formulario</t>
   </si>
   <si>
     <t>realizara la actualizacion de datos de la mascota con un Id que no Existe</t>
@@ -404,9 +386,6 @@
   </si>
   <si>
     <t>Si algún valor no es valido se debe mostrar status code 405 invalid input</t>
-  </si>
-  <si>
-    <t>CP023- Eliminar una mascota</t>
   </si>
   <si>
     <t xml:space="preserve">petId: identificador de la mascota - No existe
@@ -653,6 +632,27 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/1IajKfL2LyTfeallRPTiOz-F5Rg0GIHWY?usp=sharing</t>
+  </si>
+  <si>
+    <t>CP032- Actualizar informacion de una mascota</t>
+  </si>
+  <si>
+    <t>CP017-Agregar una nueva mascota</t>
+  </si>
+  <si>
+    <t>CP022- Filtrar mascotas por ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filtrar mascota por Status</t>
+  </si>
+  <si>
+    <t>Filtrar mascota por Status</t>
+  </si>
+  <si>
+    <t>CP033-Actualizar una mascota en la tienda con datos del formulario</t>
+  </si>
+  <si>
+    <t>Eliminar una mascota</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:AB984"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1066,7 +1066,7 @@
     <col min="9" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="13.2">
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1133,7 +1133,7 @@
         <v>34</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>26</v>
@@ -1187,7 +1187,7 @@
         <v>35</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>26</v>
@@ -1223,25 +1223,25 @@
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="I5" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>26</v>
@@ -1277,31 +1277,31 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="I6" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>27</v>
@@ -1331,31 +1331,31 @@
         <v>16</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>27</v>
@@ -1385,31 +1385,31 @@
         <v>17</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>27</v>
@@ -1439,31 +1439,31 @@
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>27</v>
@@ -1493,31 +1493,31 @@
         <v>19</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>27</v>
@@ -1547,31 +1547,31 @@
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>27</v>
@@ -1601,31 +1601,31 @@
         <v>21</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>27</v>
@@ -1655,31 +1655,31 @@
         <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>27</v>
@@ -1705,34 +1705,34 @@
     </row>
     <row r="14" spans="1:28" ht="105.6">
       <c r="B14" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>27</v>
@@ -1743,28 +1743,28 @@
     </row>
     <row r="15" spans="1:28" ht="79.2">
       <c r="B15" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>26</v>
@@ -1781,28 +1781,28 @@
     </row>
     <row r="16" spans="1:28" ht="79.2">
       <c r="B16" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="G16" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>26</v>
@@ -1819,28 +1819,28 @@
     </row>
     <row r="17" spans="2:13" ht="79.2">
       <c r="B17" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>26</v>
@@ -1857,28 +1857,28 @@
     </row>
     <row r="18" spans="2:13" ht="79.2">
       <c r="B18" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>26</v>
@@ -1895,28 +1895,28 @@
     </row>
     <row r="19" spans="2:13" ht="79.2">
       <c r="B19" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>115</v>
-      </c>
       <c r="G19" s="9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>26</v>
@@ -1933,28 +1933,28 @@
     </row>
     <row r="20" spans="2:13" ht="79.2">
       <c r="B20" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>26</v>
@@ -1971,28 +1971,28 @@
     </row>
     <row r="21" spans="2:13" ht="79.2">
       <c r="B21" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>26</v>
@@ -2009,28 +2009,28 @@
     </row>
     <row r="22" spans="2:13" ht="79.2">
       <c r="B22" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="E22" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>26</v>
@@ -2047,28 +2047,28 @@
     </row>
     <row r="23" spans="2:13" ht="79.2">
       <c r="B23" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>26</v>
@@ -2085,28 +2085,28 @@
     </row>
     <row r="24" spans="2:13" ht="79.2">
       <c r="B24" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>26</v>
@@ -2123,28 +2123,28 @@
     </row>
     <row r="25" spans="2:13" ht="79.2">
       <c r="B25" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="I25" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>26</v>
@@ -2161,28 +2161,28 @@
     </row>
     <row r="26" spans="2:13" ht="79.2">
       <c r="B26" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>26</v>
@@ -2199,28 +2199,28 @@
     </row>
     <row r="27" spans="2:13" ht="79.2">
       <c r="B27" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>26</v>
@@ -2237,28 +2237,28 @@
     </row>
     <row r="28" spans="2:13" ht="79.2">
       <c r="B28" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>26</v>
@@ -2275,28 +2275,28 @@
     </row>
     <row r="29" spans="2:13" ht="79.2">
       <c r="B29" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>26</v>
@@ -2313,28 +2313,28 @@
     </row>
     <row r="30" spans="2:13" ht="79.2">
       <c r="B30" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>26</v>
@@ -7194,19 +7194,19 @@
     <row r="3" spans="2:3">
       <c r="B3" s="13"/>
       <c r="C3" s="14" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="17"/>
       <c r="C4" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="18"/>
       <c r="C5" s="14" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>